<commit_message>
fixing some xlsx and cleaning nvessels tables
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb108/raw/Table5.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb108/raw/Table5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb108/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1185FBC-2F66-AE44-9A50-E3C5D762981C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F353E248-29E4-664B-A3BA-0434E06D572D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="580" windowWidth="25040" windowHeight="14500" xr2:uid="{C504D41A-219C-0240-BEC3-242B2C85BDD4}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{C504D41A-219C-0240-BEC3-242B2C85BDD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>25 to 39 feet</t>
   </si>
   <si>
-    <t>10 to 64 feet</t>
-  </si>
-  <si>
     <t>65 to 84 feet</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Total check</t>
+  </si>
+  <si>
+    <t>40 to 64 feet</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,27 +485,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="5">
         <v>813</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6">
         <v>731</v>

</xml_diff>